<commit_message>
added more descriptive statistics
</commit_message>
<xml_diff>
--- a/Analysis_Results/Descriptive_Analysis/descriptive_analysis.xlsx
+++ b/Analysis_Results/Descriptive_Analysis/descriptive_analysis.xlsx
@@ -1563,16 +1563,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>201930</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>168797</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>240030</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>24017</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1595,7 +1595,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="533400"/>
+          <a:off x="11010900" y="4777740"/>
           <a:ext cx="4469130" cy="3475877"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1605,25 +1605,69 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>272</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>201997</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71CF7053-2A34-4AF5-81B7-A976B5F434B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6095999" y="548912"/>
+          <a:ext cx="5078798" cy="3527788"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F118F0-C4AB-4601-96C8-5AF128DCBC01}"/>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBD64650-6D91-4944-BAE3-EDF134393DFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1631,8 +1675,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1005840" y="68580"/>
-          <a:ext cx="4000500" cy="518160"/>
+          <a:off x="6576060" y="91440"/>
+          <a:ext cx="3604260" cy="518160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1665,7 +1709,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> of Items Purchased (Both Male and Female)</a:t>
+            <a:t> of Items Purchased (Male Vs Female)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
@@ -1675,23 +1719,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>272</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>201997</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>169424</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71CF7053-2A34-4AF5-81B7-A976B5F434B2}"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A245FB-612D-4E21-B38A-64E7BC6173B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1700,15 +1744,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6095999" y="548912"/>
-          <a:ext cx="5078798" cy="3527788"/>
+          <a:off x="594360" y="4777740"/>
+          <a:ext cx="4451864" cy="3467100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1719,23 +1763,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBD64650-6D91-4944-BAE3-EDF134393DFF}"/>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1356B3F1-8A47-4D91-A3DC-5DB8B6D7BA92}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1743,8 +1787,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6576060" y="91440"/>
-          <a:ext cx="3604260" cy="518160"/>
+          <a:off x="975360" y="4312920"/>
+          <a:ext cx="4000500" cy="518160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1777,7 +1821,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> of Items Purchased (Male Vs Female)</a:t>
+            <a:t> of Items Purchased (Male)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
@@ -1787,23 +1831,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>169424</xdr:colOff>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>6126</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A245FB-612D-4E21-B38A-64E7BC6173B7}"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ABD9289-AC20-4728-87A1-A65F488E16E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1812,15 +1856,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="594360" y="4777740"/>
-          <a:ext cx="4451864" cy="3467100"/>
+          <a:off x="6103620" y="4785360"/>
+          <a:ext cx="4465320" cy="3450366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1831,23 +1875,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1356B3F1-8A47-4D91-A3DC-5DB8B6D7BA92}"/>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0CE0170-BF8E-4CD7-AE3D-EFEA3C081B9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1855,7 +1899,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="975360" y="4312920"/>
+          <a:off x="6499860" y="4305300"/>
           <a:ext cx="4000500" cy="518160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1889,7 +1933,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> of Items Purchased (Male)</a:t>
+            <a:t> of Items Purchased (Female)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
@@ -1899,23 +1943,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>6126</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>394743</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>21968</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ABD9289-AC20-4728-87A1-A65F488E16E1}"/>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D16D3CF-0410-46D8-A48B-7D42DB1D483B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1924,15 +1968,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6103620" y="4785360"/>
-          <a:ext cx="4465320" cy="3450366"/>
+          <a:off x="434340" y="320040"/>
+          <a:ext cx="4837203" cy="3725288"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1943,23 +1987,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0CE0170-BF8E-4CD7-AE3D-EFEA3C081B9B}"/>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0451B86-BCAB-49CA-A85F-AA2E1520064B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1967,8 +2011,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6499860" y="4305300"/>
-          <a:ext cx="4000500" cy="518160"/>
+          <a:off x="929640" y="76200"/>
+          <a:ext cx="3642360" cy="518160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2001,7 +2045,75 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> of Items Purchased (Female)</a:t>
+            <a:t> of Items Purchased (Both Male and Female)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34804034-4000-4719-8A93-2592645476C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11407140" y="4312920"/>
+          <a:ext cx="3992880" cy="518160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>No.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> of Items Purchased (Both Male and Female)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
@@ -4154,7 +4266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -4169,8 +4281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4184,9 +4296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V8" sqref="U8:V8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -4200,7 +4310,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>